<commit_message>
Updated cluster to the correct scores, included network graphs into the Rmd, fixed typos in the report
</commit_message>
<xml_diff>
--- a/AinBOptimisationdataModel_LF_clusters.xlsx
+++ b/AinBOptimisationdataModel_LF_clusters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="460" windowWidth="21220" windowHeight="13720"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="24520" windowHeight="13720"/>
   </bookViews>
   <sheets>
     <sheet name="Optimisation Model" sheetId="1" r:id="rId1"/>
@@ -1289,10 +1289,10 @@
   <dimension ref="A1:AG86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U9" sqref="U9"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2103,6 +2103,10 @@
       <c r="AB9" s="7" t="s">
         <v>87</v>
       </c>
+      <c r="AD9">
+        <f>SUM('Optimisation Model'!Q2:Q61)</f>
+        <v>2.6107911353700746</v>
+      </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -2190,6 +2194,10 @@
       <c r="AB10" s="7" t="s">
         <v>87</v>
       </c>
+      <c r="AD10">
+        <f>SUM('Optimisation Model'!R2:R61)</f>
+        <v>1.9843512342272998</v>
+      </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2276,6 +2284,10 @@
       </c>
       <c r="AB11" s="7" t="s">
         <v>87</v>
+      </c>
+      <c r="AD11">
+        <f>SUM('Optimisation Model'!S2:S61)</f>
+        <v>2.5509891323775657</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.2">

</xml_diff>